<commit_message>
Linear Algebra Learned By 3Blue 1Brown
</commit_message>
<xml_diff>
--- a/JANUARY/January Learnig Entries.xlsx
+++ b/JANUARY/January Learnig Entries.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>JANUARY</t>
   </si>
@@ -42,12 +42,6 @@
     <t>1. DATA TYPES,STRING
 2. TYPE CONVERSIONS
 3. INPUT AND OUTPUT</t>
-  </si>
-  <si>
-    <t>1. OPERATORS
-2.CONDITIONAL
- STATEMENTS
-3.LOOPS</t>
   </si>
   <si>
     <t>1(ARITHMETIC,
@@ -60,6 +54,19 @@
   <si>
     <t>SHERIYANS AI SCHOOL 
 https://youtu.be/_aWbUudZ5Yo?si=cohj6duDlwQ0-CI2</t>
+  </si>
+  <si>
+    <t>1. OPERATORS
+2.CONDITIONAL
+ STATEMENTS
+3.LOOPS
+4. LINEAR ALGEBRA</t>
+  </si>
+  <si>
+    <t>SHERIYANS AI SCHOOL 
+https://youtu.be/_aWbUudZ5Yo?si=cohj6duDlwQ0-CI2
+3BLUE 1BROWN
+https://youtu.be/fNk_zzaMoSs?si=4-NkCB-90DB-8J-U</t>
   </si>
 </sst>
 </file>
@@ -479,11 +486,11 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="100.8">
+    <row r="4" spans="1:6" ht="115.2">
       <c r="A4" s="2">
         <v>46359</v>
       </c>
@@ -491,13 +498,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1"/>
     </row>

</xml_diff>

<commit_message>
For loop applications on qustions Understanding
</commit_message>
<xml_diff>
--- a/JANUARY/January Learnig Entries.xlsx
+++ b/JANUARY/January Learnig Entries.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>JANUARY</t>
   </si>
@@ -42,6 +42,36 @@
     <t>1. DATA TYPES,STRING
 2. TYPE CONVERSIONS
 3. INPUT AND OUTPUT</t>
+  </si>
+  <si>
+    <t>SHERIYANS AI SCHOOL 
+https://youtu.be/_aWbUudZ5Yo?si=cohj6duDlwQ0-CI2</t>
+  </si>
+  <si>
+    <t>1. OPERATORS
+2.CONDITIONAL
+ STATEMENTS
+3.LOOPS
+4. LINEAR ALGEBRA</t>
+  </si>
+  <si>
+    <t>SHERIYANS AI SCHOOL 
+https://youtu.be/_aWbUudZ5Yo?si=cohj6duDlwQ0-CI2
+3BLUE 1BROWN
+https://youtu.be/fNk_zzaMoSs?si=4-NkCB-90DB-8J-U</t>
+  </si>
+  <si>
+    <t>1. For loop Qustions
+ solving
+ Youtube Video</t>
+  </si>
+  <si>
+    <t>1. Undrstand Application
+ for for loop to questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYTHON
+MATHS </t>
   </si>
   <si>
     <t>1(ARITHMETIC,
@@ -49,24 +79,8 @@
 COMPARISON OPERATORS,
 LOGICAL OPERATORS)
 2.(if, else,elif)
-3.(for loop , while loop with break and continue switch.)</t>
-  </si>
-  <si>
-    <t>SHERIYANS AI SCHOOL 
-https://youtu.be/_aWbUudZ5Yo?si=cohj6duDlwQ0-CI2</t>
-  </si>
-  <si>
-    <t>1. OPERATORS
-2.CONDITIONAL
- STATEMENTS
-3.LOOPS
+3.(for loop , while loop with break and continue switch.)
 4. LINEAR ALGEBRA</t>
-  </si>
-  <si>
-    <t>SHERIYANS AI SCHOOL 
-https://youtu.be/_aWbUudZ5Yo?si=cohj6duDlwQ0-CI2
-3BLUE 1BROWN
-https://youtu.be/fNk_zzaMoSs?si=4-NkCB-90DB-8J-U</t>
   </si>
 </sst>
 </file>
@@ -114,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -136,6 +150,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,14 +451,14 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="23.77734375" customWidth="1"/>
-    <col min="4" max="4" width="26.21875" customWidth="1"/>
+    <col min="4" max="4" width="43.109375" customWidth="1"/>
     <col min="5" max="5" width="23.44140625" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" customWidth="1"/>
   </cols>
@@ -486,7 +503,7 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -494,17 +511,17 @@
       <c r="A4" s="2">
         <v>46359</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>6</v>
+      <c r="B4" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -518,14 +535,22 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" ht="57.6">
       <c r="A6" s="2">
         <v>46361</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">

</xml_diff>